<commit_message>
Added Italian Yields data file
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alibenra/Desktop/Julia Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alibenra/Bocola_Dovis-2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077BD49A-BB61-3447-9F9C-367E19777E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6646B33-7B67-DC46-AE85-52AE97886470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20320" yWindow="1460" windowWidth="20320" windowHeight="14420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20320" yWindow="1460" windowWidth="20320" windowHeight="14420" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GDP" sheetId="9" r:id="rId1"/>
@@ -44488,7 +44488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AT32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+    <sheetView topLeftCell="Q1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -48996,13 +48996,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I58"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView zoomScale="51" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" s="21" customFormat="1" ht="12">
       <c r="A1" s="21" t="s">
@@ -50314,6 +50323,12 @@
     </row>
     <row r="58" spans="1:7">
       <c r="C58" s="17"/>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="C59">
+        <f>AVERAGE(C2:C51)</f>
+        <v>87.869483810787102</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>